<commit_message>
Zeiterfassung: SOLL eingetragen -> IST jeweils am Abend eintragen
</commit_message>
<xml_diff>
--- a/Zeitplanung_Janis.xlsx
+++ b/Zeitplanung_Janis.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24701"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr codeName="DieseArbeitsmappe" showPivotChartFilter="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JanisMurpf\Documents\Projekt_Blj\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\temp\projekte-ll\janis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6180890B-BDB6-4D78-B978-88ECAB0C0980}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="597" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="597"/>
   </bookViews>
   <sheets>
     <sheet name="Zeitplanung" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="1">'Ist Arbeitszeit - Übersicht'!$A$1:$O$22</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Zeitplanung!$A$1:$T$45</definedName>
   </definedNames>
-  <calcPr calcId="191029" iterate="1"/>
+  <calcPr calcId="162913" iterate="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -36,13 +35,13 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Urs Nussbaumer</author>
     <author>Benno Flory</author>
   </authors>
   <commentList>
-    <comment ref="AI7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="AI7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -56,7 +55,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AP7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+    <comment ref="AP7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -80,7 +79,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E8" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
+    <comment ref="E8" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -97,7 +96,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
+    <comment ref="P8" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -121,7 +120,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AY8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
+    <comment ref="AY8" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -135,7 +134,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AZ8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
+    <comment ref="AZ8" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -339,7 +338,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yy"/>
   </numFmts>
@@ -1645,11 +1644,11 @@
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Akzent3" xfId="1" builtinId="37"/>
-    <cellStyle name="Gelb-Feld" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Gelb-Feld" xfId="2"/>
     <cellStyle name="Prozent" xfId="5" builtinId="5"/>
-    <cellStyle name="schatten_blau" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="schatten_blau" xfId="3"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
-    <cellStyle name="Titel" xfId="4" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Titel" xfId="4"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1742,22 +1741,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>3.5</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>51</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1816,22 +1815,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>2.5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>51</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2323,26 +2322,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Tabelle1">
     <tabColor rgb="FF00B050"/>
   </sheetPr>
   <dimension ref="A1:BJ45"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="S41" sqref="S41"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.625" style="5" customWidth="1"/>
-    <col min="2" max="2" width="31.875" style="5" customWidth="1"/>
-    <col min="3" max="3" width="5.25" style="5" customWidth="1"/>
-    <col min="4" max="4" width="5.25" style="13" customWidth="1"/>
-    <col min="5" max="6" width="5.25" style="5" customWidth="1"/>
-    <col min="7" max="62" width="2.25" style="5" customWidth="1"/>
+    <col min="1" max="1" width="3.59765625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="31.8984375" style="5" customWidth="1"/>
+    <col min="3" max="3" width="5.19921875" style="5" customWidth="1"/>
+    <col min="4" max="4" width="5.19921875" style="13" customWidth="1"/>
+    <col min="5" max="6" width="5.19921875" style="5" customWidth="1"/>
+    <col min="7" max="62" width="2.19921875" style="5" customWidth="1"/>
     <col min="63" max="16384" width="12.5" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:62" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:62" ht="25.2" x14ac:dyDescent="0.3">
       <c r="A1" s="87"/>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -2374,7 +2375,7 @@
       <c r="AC1" s="4"/>
       <c r="AD1" s="4"/>
     </row>
-    <row r="2" spans="1:62" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:62" ht="5.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -2438,7 +2439,7 @@
       <c r="BI2" s="6"/>
       <c r="BJ2" s="6"/>
     </row>
-    <row r="3" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6"/>
       <c r="B3" s="6"/>
       <c r="C3" s="6"/>
@@ -2504,7 +2505,7 @@
       <c r="BI3" s="6"/>
       <c r="BJ3" s="6"/>
     </row>
-    <row r="4" spans="1:62" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:62" ht="6.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6"/>
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
@@ -2568,7 +2569,7 @@
       <c r="BI4" s="6"/>
       <c r="BJ4" s="6"/>
     </row>
-    <row r="5" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
@@ -2634,7 +2635,7 @@
       <c r="BI5" s="6"/>
       <c r="BJ5" s="6"/>
     </row>
-    <row r="6" spans="1:62" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:62" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="7"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -2642,7 +2643,7 @@
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="1:62" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:62" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="9"/>
       <c r="B7" s="26"/>
       <c r="C7" s="114" t="s">
@@ -2728,7 +2729,7 @@
       <c r="BI7" s="115"/>
       <c r="BJ7" s="118"/>
     </row>
-    <row r="8" spans="1:62" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:62" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
         <v>0</v>
       </c>
@@ -2914,7 +2915,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="29">
         <v>10</v>
       </c>
@@ -2923,11 +2924,11 @@
       </c>
       <c r="C9" s="40">
         <f>SUM(C10:C13)</f>
-        <v>3.5</v>
+        <v>6</v>
       </c>
       <c r="D9" s="41">
         <f>SUM(D10:D13)</f>
-        <v>2.5</v>
+        <v>0</v>
       </c>
       <c r="E9" s="31"/>
       <c r="F9" s="30"/>
@@ -2988,7 +2989,7 @@
       <c r="BI9" s="71"/>
       <c r="BJ9" s="75"/>
     </row>
-    <row r="10" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="12">
         <v>101</v>
       </c>
@@ -3075,7 +3076,7 @@
       <c r="BI10" s="56"/>
       <c r="BJ10" s="57"/>
     </row>
-    <row r="11" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="11">
         <v>102</v>
       </c>
@@ -3152,17 +3153,19 @@
       <c r="BI11" s="56"/>
       <c r="BJ11" s="57"/>
     </row>
-    <row r="12" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="11">
         <v>103</v>
       </c>
       <c r="B12" s="44" t="s">
         <v>38</v>
       </c>
-      <c r="C12" s="48"/>
+      <c r="C12" s="48">
+        <v>2.5</v>
+      </c>
       <c r="D12" s="80">
         <f t="shared" ref="D12:D13" si="0">SUM(G12:BJ12)</f>
-        <v>2.5</v>
+        <v>0</v>
       </c>
       <c r="E12" s="49">
         <v>1</v>
@@ -3172,34 +3175,26 @@
       <c r="H12" s="59"/>
       <c r="I12" s="60"/>
       <c r="J12" s="60"/>
-      <c r="K12" s="104">
-        <v>0.5</v>
-      </c>
+      <c r="K12" s="104"/>
       <c r="L12" s="56"/>
       <c r="M12" s="57"/>
       <c r="N12" s="58"/>
       <c r="O12" s="59"/>
       <c r="P12" s="59"/>
       <c r="Q12" s="60"/>
-      <c r="R12" s="104">
-        <v>0.5</v>
-      </c>
+      <c r="R12" s="104"/>
       <c r="S12" s="56"/>
       <c r="T12" s="57"/>
       <c r="U12" s="58"/>
       <c r="V12" s="59"/>
       <c r="W12" s="60"/>
       <c r="X12" s="60"/>
-      <c r="Y12" s="104">
-        <v>0.5</v>
-      </c>
+      <c r="Y12" s="104"/>
       <c r="Z12" s="56"/>
       <c r="AA12" s="57"/>
       <c r="AB12" s="98"/>
       <c r="AC12" s="60"/>
-      <c r="AD12" s="103">
-        <v>0.5</v>
-      </c>
+      <c r="AD12" s="103"/>
       <c r="AE12" s="59"/>
       <c r="AF12" s="89"/>
       <c r="AG12" s="56"/>
@@ -3222,9 +3217,7 @@
       <c r="AX12" s="59"/>
       <c r="AY12" s="59"/>
       <c r="AZ12" s="59"/>
-      <c r="BA12" s="104">
-        <v>0.5</v>
-      </c>
+      <c r="BA12" s="104"/>
       <c r="BB12" s="56"/>
       <c r="BC12" s="57"/>
       <c r="BD12" s="58"/>
@@ -3235,7 +3228,7 @@
       <c r="BI12" s="56"/>
       <c r="BJ12" s="57"/>
     </row>
-    <row r="13" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="11">
         <v>104</v>
       </c>
@@ -3312,7 +3305,7 @@
       <c r="BI13" s="64"/>
       <c r="BJ13" s="65"/>
     </row>
-    <row r="14" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="29">
         <v>20</v>
       </c>
@@ -3386,7 +3379,7 @@
       <c r="BI14" s="71"/>
       <c r="BJ14" s="75"/>
     </row>
-    <row r="15" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="12">
         <v>201</v>
       </c>
@@ -3465,7 +3458,7 @@
       <c r="BI15" s="56"/>
       <c r="BJ15" s="57"/>
     </row>
-    <row r="16" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="12">
         <v>202</v>
       </c>
@@ -3542,7 +3535,7 @@
       <c r="BI16" s="56"/>
       <c r="BJ16" s="57"/>
     </row>
-    <row r="17" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="12">
         <v>203</v>
       </c>
@@ -3611,7 +3604,7 @@
       <c r="BI17" s="56"/>
       <c r="BJ17" s="57"/>
     </row>
-    <row r="18" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="29">
         <v>30</v>
       </c>
@@ -3620,11 +3613,11 @@
       </c>
       <c r="C18" s="40">
         <f>SUM(C19:C33)</f>
-        <v>0</v>
+        <v>51</v>
       </c>
       <c r="D18" s="41">
         <f>SUM(D19:D33)</f>
-        <v>51</v>
+        <v>9</v>
       </c>
       <c r="E18" s="31"/>
       <c r="F18" s="30"/>
@@ -3685,14 +3678,16 @@
       <c r="BI18" s="71"/>
       <c r="BJ18" s="75"/>
     </row>
-    <row r="19" spans="1:62" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:62" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A19" s="12">
         <v>301</v>
       </c>
       <c r="B19" s="95" t="s">
         <v>49</v>
       </c>
-      <c r="C19" s="48"/>
+      <c r="C19" s="48">
+        <v>5</v>
+      </c>
       <c r="D19" s="80">
         <f t="shared" ref="D19:D33" si="1">SUM(G19:BJ19)</f>
         <v>5</v>
@@ -3762,14 +3757,16 @@
       <c r="BI19" s="56"/>
       <c r="BJ19" s="57"/>
     </row>
-    <row r="20" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="12">
         <v>302</v>
       </c>
       <c r="B20" s="45" t="s">
         <v>43</v>
       </c>
-      <c r="C20" s="48"/>
+      <c r="C20" s="48">
+        <v>4</v>
+      </c>
       <c r="D20" s="80">
         <f t="shared" si="1"/>
         <v>4</v>
@@ -3837,17 +3834,19 @@
       <c r="BI20" s="56"/>
       <c r="BJ20" s="57"/>
     </row>
-    <row r="21" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="12">
         <v>303</v>
       </c>
       <c r="B21" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="C21" s="48"/>
+      <c r="C21" s="48">
+        <v>4</v>
+      </c>
       <c r="D21" s="80">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E21" s="49">
         <v>1</v>
@@ -3869,9 +3868,7 @@
       <c r="T21" s="57"/>
       <c r="U21" s="58"/>
       <c r="V21" s="59"/>
-      <c r="W21" s="86">
-        <v>4</v>
-      </c>
+      <c r="W21" s="86"/>
       <c r="X21" s="54"/>
       <c r="Y21" s="55"/>
       <c r="Z21" s="56"/>
@@ -3912,17 +3909,19 @@
       <c r="BI21" s="56"/>
       <c r="BJ21" s="57"/>
     </row>
-    <row r="22" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="12">
         <v>304</v>
       </c>
       <c r="B22" s="45" t="s">
         <v>53</v>
       </c>
-      <c r="C22" s="48"/>
+      <c r="C22" s="48">
+        <v>4</v>
+      </c>
       <c r="D22" s="80">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E22" s="49">
         <v>1</v>
@@ -3944,9 +3943,7 @@
       <c r="T22" s="57"/>
       <c r="U22" s="58"/>
       <c r="V22" s="59"/>
-      <c r="W22" s="86">
-        <v>4</v>
-      </c>
+      <c r="W22" s="86"/>
       <c r="X22" s="54"/>
       <c r="Y22" s="55"/>
       <c r="Z22" s="56"/>
@@ -3987,17 +3984,19 @@
       <c r="BI22" s="56"/>
       <c r="BJ22" s="57"/>
     </row>
-    <row r="23" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="12">
         <v>305</v>
       </c>
       <c r="B23" s="45" t="s">
         <v>52</v>
       </c>
-      <c r="C23" s="48"/>
+      <c r="C23" s="48">
+        <v>10</v>
+      </c>
       <c r="D23" s="80">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E23" s="49">
         <v>1</v>
@@ -4020,12 +4019,8 @@
       <c r="U23" s="58"/>
       <c r="V23" s="59"/>
       <c r="W23" s="60"/>
-      <c r="X23" s="108">
-        <v>8</v>
-      </c>
-      <c r="Y23" s="106">
-        <v>2</v>
-      </c>
+      <c r="X23" s="108"/>
+      <c r="Y23" s="106"/>
       <c r="Z23" s="56"/>
       <c r="AA23" s="57"/>
       <c r="AB23" s="98"/>
@@ -4064,17 +4059,19 @@
       <c r="BI23" s="56"/>
       <c r="BJ23" s="57"/>
     </row>
-    <row r="24" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="12">
         <v>306</v>
       </c>
       <c r="B24" s="45" t="s">
         <v>59</v>
       </c>
-      <c r="C24" s="48"/>
+      <c r="C24" s="48">
+        <v>9</v>
+      </c>
       <c r="D24" s="80">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="E24" s="49"/>
       <c r="F24" s="50"/>
@@ -4099,12 +4096,8 @@
       <c r="Y24" s="55"/>
       <c r="Z24" s="56"/>
       <c r="AA24" s="57"/>
-      <c r="AB24" s="109">
-        <v>6</v>
-      </c>
-      <c r="AC24" s="108">
-        <v>3</v>
-      </c>
+      <c r="AB24" s="109"/>
+      <c r="AC24" s="108"/>
       <c r="AD24" s="107"/>
       <c r="AE24" s="88"/>
       <c r="AF24" s="89"/>
@@ -4139,17 +4132,19 @@
       <c r="BI24" s="56"/>
       <c r="BJ24" s="57"/>
     </row>
-    <row r="25" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="12">
         <v>307</v>
       </c>
       <c r="B25" s="45" t="s">
         <v>54</v>
       </c>
-      <c r="C25" s="48"/>
+      <c r="C25" s="48">
+        <v>4</v>
+      </c>
       <c r="D25" s="80">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E25" s="49"/>
       <c r="F25" s="50"/>
@@ -4171,9 +4166,7 @@
       <c r="V25" s="59"/>
       <c r="W25" s="54"/>
       <c r="X25" s="54"/>
-      <c r="Y25" s="106">
-        <v>4</v>
-      </c>
+      <c r="Y25" s="106"/>
       <c r="Z25" s="56"/>
       <c r="AA25" s="57"/>
       <c r="AB25" s="110"/>
@@ -4212,17 +4205,19 @@
       <c r="BI25" s="56"/>
       <c r="BJ25" s="57"/>
     </row>
-    <row r="26" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="12">
         <v>308</v>
       </c>
       <c r="B26" s="45" t="s">
         <v>55</v>
       </c>
-      <c r="C26" s="48"/>
+      <c r="C26" s="48">
+        <v>4</v>
+      </c>
       <c r="D26" s="80">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E26" s="49"/>
       <c r="F26" s="50"/>
@@ -4244,14 +4239,10 @@
       <c r="V26" s="59"/>
       <c r="W26" s="54"/>
       <c r="X26" s="54"/>
-      <c r="Y26" s="106">
-        <v>2</v>
-      </c>
+      <c r="Y26" s="106"/>
       <c r="Z26" s="56"/>
       <c r="AA26" s="57"/>
-      <c r="AB26" s="109">
-        <v>2</v>
-      </c>
+      <c r="AB26" s="109"/>
       <c r="AC26" s="81"/>
       <c r="AD26" s="54"/>
       <c r="AE26" s="88"/>
@@ -4287,17 +4278,19 @@
       <c r="BI26" s="56"/>
       <c r="BJ26" s="57"/>
     </row>
-    <row r="27" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="12">
         <v>309</v>
       </c>
       <c r="B27" s="45" t="s">
         <v>56</v>
       </c>
-      <c r="C27" s="48"/>
+      <c r="C27" s="48">
+        <v>2</v>
+      </c>
       <c r="D27" s="80">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E27" s="49"/>
       <c r="F27" s="50"/>
@@ -4323,9 +4316,7 @@
       <c r="Z27" s="56"/>
       <c r="AA27" s="57"/>
       <c r="AB27" s="98"/>
-      <c r="AC27" s="108">
-        <v>2</v>
-      </c>
+      <c r="AC27" s="108"/>
       <c r="AD27" s="107"/>
       <c r="AE27" s="88"/>
       <c r="AF27" s="89"/>
@@ -4360,17 +4351,19 @@
       <c r="BI27" s="56"/>
       <c r="BJ27" s="57"/>
     </row>
-    <row r="28" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="12">
         <v>310</v>
       </c>
       <c r="B28" s="45" t="s">
         <v>57</v>
       </c>
-      <c r="C28" s="48"/>
+      <c r="C28" s="48">
+        <v>2</v>
+      </c>
       <c r="D28" s="80">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E28" s="49"/>
       <c r="F28" s="50"/>
@@ -4396,9 +4389,7 @@
       <c r="Z28" s="56"/>
       <c r="AA28" s="57"/>
       <c r="AB28" s="98"/>
-      <c r="AC28" s="108">
-        <v>2</v>
-      </c>
+      <c r="AC28" s="108"/>
       <c r="AD28" s="107"/>
       <c r="AE28" s="88"/>
       <c r="AF28" s="89"/>
@@ -4433,17 +4424,19 @@
       <c r="BI28" s="56"/>
       <c r="BJ28" s="57"/>
     </row>
-    <row r="29" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="12">
         <v>311</v>
       </c>
       <c r="B29" s="45" t="s">
         <v>58</v>
       </c>
-      <c r="C29" s="48"/>
+      <c r="C29" s="48">
+        <v>3</v>
+      </c>
       <c r="D29" s="80">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E29" s="49"/>
       <c r="F29" s="50"/>
@@ -4469,12 +4462,8 @@
       <c r="Z29" s="56"/>
       <c r="AA29" s="57"/>
       <c r="AB29" s="101"/>
-      <c r="AC29" s="111">
-        <v>1</v>
-      </c>
-      <c r="AD29" s="86">
-        <v>2</v>
-      </c>
+      <c r="AC29" s="111"/>
+      <c r="AD29" s="86"/>
       <c r="AE29" s="88"/>
       <c r="AF29" s="89"/>
       <c r="AG29" s="56"/>
@@ -4508,7 +4497,7 @@
       <c r="BI29" s="56"/>
       <c r="BJ29" s="57"/>
     </row>
-    <row r="30" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="12">
         <v>312</v>
       </c>
@@ -4577,7 +4566,7 @@
       <c r="BI30" s="56"/>
       <c r="BJ30" s="57"/>
     </row>
-    <row r="31" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="12">
         <v>313</v>
       </c>
@@ -4646,7 +4635,7 @@
       <c r="BI31" s="56"/>
       <c r="BJ31" s="57"/>
     </row>
-    <row r="32" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="12">
         <v>314</v>
       </c>
@@ -4715,7 +4704,7 @@
       <c r="BI32" s="56"/>
       <c r="BJ32" s="57"/>
     </row>
-    <row r="33" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="12">
         <v>315</v>
       </c>
@@ -4784,7 +4773,7 @@
       <c r="BI33" s="56"/>
       <c r="BJ33" s="57"/>
     </row>
-    <row r="34" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="29">
         <v>40</v>
       </c>
@@ -4793,11 +4782,11 @@
       </c>
       <c r="C34" s="40">
         <f>SUM(C35:C37)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D34" s="41">
         <f>SUM(D35:D37)</f>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E34" s="31"/>
       <c r="F34" s="30"/>
@@ -4858,17 +4847,19 @@
       <c r="BI34" s="71"/>
       <c r="BJ34" s="75"/>
     </row>
-    <row r="35" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="12">
         <v>401</v>
       </c>
       <c r="B35" s="45" t="s">
         <v>21</v>
       </c>
-      <c r="C35" s="48"/>
+      <c r="C35" s="48">
+        <v>1</v>
+      </c>
       <c r="D35" s="80">
         <f t="shared" ref="D35:D37" si="2">SUM(G35:BJ35)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E35" s="49"/>
       <c r="F35" s="50"/>
@@ -4895,9 +4886,7 @@
       <c r="AA35" s="57"/>
       <c r="AB35" s="96"/>
       <c r="AC35" s="97"/>
-      <c r="AD35" s="112">
-        <v>1</v>
-      </c>
+      <c r="AD35" s="112"/>
       <c r="AE35" s="88"/>
       <c r="AF35" s="89"/>
       <c r="AG35" s="56"/>
@@ -4931,17 +4920,19 @@
       <c r="BI35" s="56"/>
       <c r="BJ35" s="57"/>
     </row>
-    <row r="36" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="12">
         <v>402</v>
       </c>
       <c r="B36" s="45" t="s">
         <v>23</v>
       </c>
-      <c r="C36" s="48"/>
+      <c r="C36" s="48">
+        <v>2</v>
+      </c>
       <c r="D36" s="80">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E36" s="49"/>
       <c r="F36" s="50"/>
@@ -4968,9 +4959,7 @@
       <c r="AA36" s="57"/>
       <c r="AB36" s="98"/>
       <c r="AC36" s="60"/>
-      <c r="AD36" s="112">
-        <v>2</v>
-      </c>
+      <c r="AD36" s="112"/>
       <c r="AE36" s="88"/>
       <c r="AF36" s="89"/>
       <c r="AG36" s="56"/>
@@ -5004,17 +4993,19 @@
       <c r="BI36" s="56"/>
       <c r="BJ36" s="57"/>
     </row>
-    <row r="37" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="12">
         <v>403</v>
       </c>
       <c r="B37" s="45" t="s">
         <v>22</v>
       </c>
-      <c r="C37" s="48"/>
+      <c r="C37" s="48">
+        <v>3</v>
+      </c>
       <c r="D37" s="80">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E37" s="49"/>
       <c r="F37" s="50"/>
@@ -5041,9 +5032,7 @@
       <c r="AA37" s="57"/>
       <c r="AB37" s="98"/>
       <c r="AC37" s="60"/>
-      <c r="AD37" s="112">
-        <v>3</v>
-      </c>
+      <c r="AD37" s="112"/>
       <c r="AE37" s="88"/>
       <c r="AF37" s="89"/>
       <c r="AG37" s="56"/>
@@ -5077,7 +5066,7 @@
       <c r="BI37" s="56"/>
       <c r="BJ37" s="57"/>
     </row>
-    <row r="38" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="29">
         <v>50</v>
       </c>
@@ -5090,7 +5079,7 @@
       </c>
       <c r="D38" s="41">
         <f>SUM(D39:D40)</f>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E38" s="31"/>
       <c r="F38" s="30"/>
@@ -5151,7 +5140,7 @@
       <c r="BI38" s="71"/>
       <c r="BJ38" s="75"/>
     </row>
-    <row r="39" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="12">
         <v>501</v>
       </c>
@@ -5161,7 +5150,7 @@
       <c r="C39" s="48"/>
       <c r="D39" s="80">
         <f>SUM(G39:BJ39)</f>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E39" s="49"/>
       <c r="F39" s="50"/>
@@ -5211,9 +5200,7 @@
       <c r="AX39" s="53"/>
       <c r="AY39" s="88"/>
       <c r="AZ39" s="88"/>
-      <c r="BA39" s="113">
-        <v>6</v>
-      </c>
+      <c r="BA39" s="113"/>
       <c r="BB39" s="56"/>
       <c r="BC39" s="57"/>
       <c r="BD39" s="52"/>
@@ -5224,7 +5211,7 @@
       <c r="BI39" s="56"/>
       <c r="BJ39" s="57"/>
     </row>
-    <row r="40" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="12">
         <v>502</v>
       </c>
@@ -5293,7 +5280,7 @@
       <c r="BI40" s="56"/>
       <c r="BJ40" s="57"/>
     </row>
-    <row r="41" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="29">
         <v>60</v>
       </c>
@@ -5302,11 +5289,11 @@
       </c>
       <c r="C41" s="40">
         <f>SUM(C42:C44)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D41" s="41">
         <f>SUM(D42:D44)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E41" s="31"/>
       <c r="F41" s="30"/>
@@ -5367,17 +5354,19 @@
       <c r="BI41" s="71"/>
       <c r="BJ41" s="75"/>
     </row>
-    <row r="42" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="12">
         <v>601</v>
       </c>
       <c r="B42" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="C42" s="48"/>
+      <c r="C42" s="48">
+        <v>1</v>
+      </c>
       <c r="D42" s="80">
         <f t="shared" ref="D42:D44" si="3">SUM(G42:BJ42)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E42" s="49"/>
       <c r="F42" s="50"/>
@@ -5427,9 +5416,7 @@
       <c r="AX42" s="53"/>
       <c r="AY42" s="88"/>
       <c r="AZ42" s="88"/>
-      <c r="BA42" s="113">
-        <v>1</v>
-      </c>
+      <c r="BA42" s="113"/>
       <c r="BB42" s="56"/>
       <c r="BC42" s="57"/>
       <c r="BD42" s="52"/>
@@ -5440,17 +5427,19 @@
       <c r="BI42" s="56"/>
       <c r="BJ42" s="57"/>
     </row>
-    <row r="43" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="12">
         <v>602</v>
       </c>
       <c r="B43" s="45" t="s">
         <v>40</v>
       </c>
-      <c r="C43" s="48"/>
+      <c r="C43" s="48">
+        <v>1</v>
+      </c>
       <c r="D43" s="80">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E43" s="49"/>
       <c r="F43" s="50"/>
@@ -5500,9 +5489,7 @@
       <c r="AX43" s="59"/>
       <c r="AY43" s="88"/>
       <c r="AZ43" s="88"/>
-      <c r="BA43" s="113">
-        <v>1</v>
-      </c>
+      <c r="BA43" s="113"/>
       <c r="BB43" s="56"/>
       <c r="BC43" s="57"/>
       <c r="BD43" s="58"/>
@@ -5513,7 +5500,7 @@
       <c r="BI43" s="56"/>
       <c r="BJ43" s="57"/>
     </row>
-    <row r="44" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="12">
         <v>603</v>
       </c>
@@ -5582,18 +5569,18 @@
       <c r="BI44" s="56"/>
       <c r="BJ44" s="57"/>
     </row>
-    <row r="45" spans="1:62" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:62" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="34"/>
       <c r="B45" s="35" t="s">
         <v>6</v>
       </c>
       <c r="C45" s="36">
         <f>C41+C38+C34+C18+C14+C9</f>
-        <v>11.5</v>
+        <v>73</v>
       </c>
       <c r="D45" s="36">
         <f>D41+D38+D34+D18+D14+D9</f>
-        <v>73.5</v>
+        <v>15</v>
       </c>
       <c r="E45" s="36"/>
       <c r="F45" s="37"/>
@@ -5615,7 +5602,7 @@
       </c>
       <c r="K45" s="38">
         <f t="shared" si="4"/>
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="L45" s="38">
         <f t="shared" si="4"/>
@@ -5643,7 +5630,7 @@
       </c>
       <c r="R45" s="38">
         <f t="shared" si="4"/>
-        <v>7.5</v>
+        <v>7</v>
       </c>
       <c r="S45" s="38">
         <f t="shared" si="4"/>
@@ -5663,15 +5650,15 @@
       </c>
       <c r="W45" s="38">
         <f t="shared" si="4"/>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="X45" s="38">
         <f t="shared" si="4"/>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="Y45" s="38">
         <f t="shared" si="4"/>
-        <v>8.5</v>
+        <v>0</v>
       </c>
       <c r="Z45" s="38">
         <f t="shared" si="4"/>
@@ -5683,15 +5670,15 @@
       </c>
       <c r="AB45" s="38">
         <f t="shared" si="4"/>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="AC45" s="38">
         <f t="shared" si="4"/>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="AD45" s="38">
         <f t="shared" si="4"/>
-        <v>8.5</v>
+        <v>0</v>
       </c>
       <c r="AE45" s="38">
         <f t="shared" si="4"/>
@@ -5783,7 +5770,7 @@
       </c>
       <c r="BA45" s="38">
         <f t="shared" si="5"/>
-        <v>8.5</v>
+        <v>0</v>
       </c>
       <c r="BB45" s="38">
         <f t="shared" si="5"/>
@@ -5847,7 +5834,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Tabelle2">
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
@@ -5857,17 +5844,17 @@
       <selection activeCell="P20" sqref="P20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="13.09765625" style="1" customWidth="1"/>
     <col min="2" max="2" width="12.5" style="2" customWidth="1"/>
     <col min="3" max="3" width="13.5" style="1" customWidth="1"/>
-    <col min="4" max="4" width="9.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.19921875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:6" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:6" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="121" t="s">
         <v>12</v>
       </c>
@@ -5879,7 +5866,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="16.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="119" t="str">
         <f>Zeitplanung!B9</f>
         <v>Administration, Planung</v>
@@ -5887,16 +5874,16 @@
       <c r="B3" s="120"/>
       <c r="C3" s="77">
         <f>Zeitplanung!C9</f>
-        <v>3.5</v>
+        <v>6</v>
       </c>
       <c r="D3" s="77">
         <f>Zeitplanung!D9</f>
-        <v>2.5</v>
+        <v>0</v>
       </c>
       <c r="E3" s="79"/>
       <c r="F3" s="78"/>
     </row>
-    <row r="4" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="16.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="119" t="str">
         <f>Zeitplanung!B14</f>
         <v>Analyse &amp; Design</v>
@@ -5913,7 +5900,7 @@
       <c r="E4" s="79"/>
       <c r="F4" s="78"/>
     </row>
-    <row r="5" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="16.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="119" t="str">
         <f>Zeitplanung!B18</f>
         <v>Implementation</v>
@@ -5921,16 +5908,16 @@
       <c r="B5" s="120"/>
       <c r="C5" s="77">
         <f>Zeitplanung!C18</f>
-        <v>0</v>
+        <v>51</v>
       </c>
       <c r="D5" s="77">
         <f>Zeitplanung!D18</f>
-        <v>51</v>
+        <v>9</v>
       </c>
       <c r="E5" s="79"/>
       <c r="F5" s="78"/>
     </row>
-    <row r="6" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="16.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="119" t="str">
         <f>Zeitplanung!B34</f>
         <v>Testen</v>
@@ -5938,15 +5925,15 @@
       <c r="B6" s="120"/>
       <c r="C6" s="77">
         <f>Zeitplanung!C34</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D6" s="77">
         <f>Zeitplanung!D34</f>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="F6" s="78"/>
     </row>
-    <row r="7" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="16.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="119" t="str">
         <f>Zeitplanung!B38</f>
         <v>Diverses</v>
@@ -5958,11 +5945,11 @@
       </c>
       <c r="D7" s="77">
         <f>Zeitplanung!D38</f>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="F7" s="78"/>
     </row>
-    <row r="8" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="16.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="119" t="str">
         <f>Zeitplanung!B41</f>
         <v>Abschluss</v>
@@ -5970,15 +5957,15 @@
       <c r="B8" s="120"/>
       <c r="C8" s="77">
         <f>Zeitplanung!C41</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D8" s="77">
         <f>Zeitplanung!D41</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F8" s="78"/>
     </row>
-    <row r="9" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="9" spans="1:6" ht="15.6" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="7">
     <mergeCell ref="A7:B7"/>

</xml_diff>